<commit_message>
change ps in action3
</commit_message>
<xml_diff>
--- a/data/action3/test1/1/data.xlsx
+++ b/data/action3/test1/1/data.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -397,12 +397,12 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>boy</v>
+        <v>girl</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>boy</v>
+        <v>girl</v>
       </c>
     </row>
     <row r="6">
@@ -427,7 +427,7 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>boy</v>
+        <v>girl</v>
       </c>
     </row>
     <row r="11">
@@ -435,9 +435,459 @@
         <v>girl</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>boy</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>boy</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>boy</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>boy</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>boy</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>boy</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>boy</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>boy</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>boy</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>boy</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>girl</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>girl</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A101"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>